<commit_message>
features spreadsheet updated with beanie
</commit_message>
<xml_diff>
--- a/template/features.xlsx
+++ b/template/features.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pixel\Desktop\Lectures\Semester_2\Signal_image_processing\Homeworks\ImageProcessing_TeamProject\template\head\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pixel\Desktop\Lectures\Semester_2\Signal_image_processing\Homeworks\ImageProcessing_TeamProject\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="29">
   <si>
     <t>Image</t>
   </si>
@@ -98,10 +98,19 @@
     <t>Head without hair / width</t>
   </si>
   <si>
-    <t>Pick</t>
-  </si>
-  <si>
-    <t>x</t>
+    <t>Diameter pompom (only red part)</t>
+  </si>
+  <si>
+    <t>White stripe thickness</t>
+  </si>
+  <si>
+    <t>Red stripe thickness</t>
+  </si>
+  <si>
+    <t>Black separation</t>
+  </si>
+  <si>
+    <t>Angle beanie (compared to horizontal, always tilted in same direction)</t>
   </si>
 </sst>
 </file>
@@ -160,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -177,6 +186,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,11 +513,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,14 +525,15 @@
     <col min="1" max="6" width="25.77734375" customWidth="1"/>
     <col min="7" max="7" width="21.33203125" customWidth="1"/>
     <col min="8" max="8" width="25.77734375" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="31.44140625" customWidth="1"/>
-    <col min="13" max="13" width="0.44140625" customWidth="1"/>
-    <col min="14" max="14" width="35.77734375" customWidth="1"/>
+    <col min="9" max="9" width="20.21875" customWidth="1"/>
+    <col min="10" max="10" width="46.109375" customWidth="1"/>
+    <col min="11" max="13" width="30.88671875" customWidth="1"/>
+    <col min="14" max="14" width="17.109375" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" customWidth="1"/>
+    <col min="16" max="16" width="35.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -536,23 +558,36 @@
       <c r="H1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="T1" s="6"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -577,21 +612,36 @@
       <c r="H2" s="5">
         <v>6</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="K2">
+      <c r="I2" s="8">
+        <v>60</v>
+      </c>
+      <c r="J2" s="8">
+        <v>3.6</v>
+      </c>
+      <c r="K2" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="L2" s="8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M2" s="8">
+        <v>1</v>
+      </c>
+      <c r="N2" s="5"/>
+      <c r="P2">
         <f>F2/G2</f>
         <v>1.5</v>
       </c>
-      <c r="L2">
+      <c r="Q2">
         <f>4*F2</f>
         <v>12</v>
       </c>
-      <c r="N2">
+      <c r="S2">
         <f>C2/D2</f>
         <v>1.1666666666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -616,21 +666,38 @@
       <c r="H3" s="5">
         <v>4</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="K3">
-        <f t="shared" ref="K3:K24" si="0">F3/G3</f>
+      <c r="I3" s="8">
+        <v>35</v>
+      </c>
+      <c r="J3" s="8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K3" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="L3" s="8">
+        <v>1.6</v>
+      </c>
+      <c r="M3" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3">
+        <f>F3/G3</f>
         <v>1</v>
       </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L24" si="1">4*F3</f>
+      <c r="Q3">
+        <f>4*F3</f>
         <v>12</v>
       </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N24" si="2">C3/D3</f>
+      <c r="S3">
+        <f>C3/D3</f>
         <v>1.2727272727272727</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -655,21 +722,36 @@
       <c r="H4" s="5">
         <v>2</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="K4">
-        <f t="shared" si="0"/>
+      <c r="I4" s="8">
+        <v>45</v>
+      </c>
+      <c r="J4" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="K4" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="L4" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="M4" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="P4">
+        <f>F4/G4</f>
         <v>1</v>
       </c>
-      <c r="L4">
-        <f t="shared" si="1"/>
+      <c r="Q4">
+        <f>4*F4</f>
         <v>12</v>
       </c>
-      <c r="N4">
-        <f t="shared" si="2"/>
+      <c r="S4">
+        <f>C4/D4</f>
         <v>1.4545454545454546</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -694,21 +776,36 @@
       <c r="H5" s="5">
         <v>7</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="K5">
-        <f t="shared" si="0"/>
+      <c r="I5" s="8">
+        <v>42</v>
+      </c>
+      <c r="J5" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="K5" s="8">
+        <v>2.4</v>
+      </c>
+      <c r="L5" s="8">
+        <v>2.6</v>
+      </c>
+      <c r="M5" s="8">
+        <v>1</v>
+      </c>
+      <c r="N5" s="5"/>
+      <c r="P5">
+        <f>F5/G5</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="L5">
-        <f t="shared" si="1"/>
+      <c r="Q5">
+        <f>4*F5</f>
         <v>16</v>
       </c>
-      <c r="N5">
-        <f t="shared" si="2"/>
+      <c r="S5">
+        <f>C5/D5</f>
         <v>1.6</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -733,24 +830,36 @@
       <c r="H6" s="5">
         <v>8</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="K6">
-        <f t="shared" si="0"/>
+      <c r="I6" s="8">
+        <v>45</v>
+      </c>
+      <c r="J6" s="8">
+        <v>4</v>
+      </c>
+      <c r="K6" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="L6" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="M6" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N6" s="5"/>
+      <c r="P6">
+        <f>F6/G6</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="L6">
-        <f t="shared" si="1"/>
+      <c r="Q6">
+        <f>4*F6</f>
         <v>16</v>
       </c>
-      <c r="N6">
-        <f t="shared" si="2"/>
+      <c r="S6">
+        <f>C6/D6</f>
         <v>1.5714285714285714</v>
       </c>
-      <c r="O6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -775,23 +884,38 @@
       <c r="H7" s="5">
         <v>9</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="8">
+        <v>0</v>
+      </c>
+      <c r="J7" s="8">
+        <v>5</v>
+      </c>
+      <c r="K7" s="8">
+        <v>2</v>
+      </c>
+      <c r="L7" s="8">
+        <v>5</v>
+      </c>
+      <c r="M7" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="N7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
+      <c r="P7">
+        <f>F7/G7</f>
         <v>1.2</v>
       </c>
-      <c r="L7">
-        <f t="shared" si="1"/>
+      <c r="Q7">
+        <f>4*F7</f>
         <v>24</v>
       </c>
-      <c r="N7">
-        <f t="shared" si="2"/>
+      <c r="S7">
+        <f>C7/D7</f>
         <v>1.4615384615384615</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -816,14 +940,29 @@
       <c r="H8" s="5">
         <v>6</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="8">
+        <v>45</v>
+      </c>
+      <c r="J8" s="8">
+        <v>7</v>
+      </c>
+      <c r="K8" s="8">
+        <v>5</v>
+      </c>
+      <c r="L8" s="8">
+        <v>4</v>
+      </c>
+      <c r="M8" s="8">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L8">
+      <c r="Q8">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -848,11 +987,26 @@
       <c r="H9" s="5">
         <v>5</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -877,17 +1031,32 @@
       <c r="H10" s="5">
         <v>6</v>
       </c>
-      <c r="I10" s="5"/>
-      <c r="L10">
-        <f t="shared" si="1"/>
+      <c r="I10" s="8">
+        <v>68</v>
+      </c>
+      <c r="J10" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="K10" s="8">
+        <v>2</v>
+      </c>
+      <c r="L10" s="8">
+        <v>2</v>
+      </c>
+      <c r="M10" s="8">
+        <v>1</v>
+      </c>
+      <c r="N10" s="5"/>
+      <c r="Q10">
+        <f>4*F10</f>
         <v>16</v>
       </c>
-      <c r="N10">
-        <f t="shared" si="2"/>
+      <c r="S10">
+        <f>C10/D10</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -912,21 +1081,36 @@
       <c r="H11" s="5">
         <v>9</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="K11">
-        <f t="shared" si="0"/>
+      <c r="I11" s="8">
+        <v>68</v>
+      </c>
+      <c r="J11" s="8">
+        <v>3.2</v>
+      </c>
+      <c r="K11" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="L11" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="M11" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="N11" s="5"/>
+      <c r="P11">
+        <f>F11/G11</f>
         <v>1</v>
       </c>
-      <c r="L11">
-        <f t="shared" si="1"/>
+      <c r="Q11">
+        <f>4*F11</f>
         <v>12</v>
       </c>
-      <c r="N11">
-        <f t="shared" si="2"/>
+      <c r="S11">
+        <f>C11/D11</f>
         <v>1.375</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -951,21 +1135,36 @@
       <c r="H12" s="5">
         <v>8</v>
       </c>
-      <c r="I12" s="5"/>
-      <c r="K12">
-        <f t="shared" si="0"/>
+      <c r="I12" s="8">
+        <v>45</v>
+      </c>
+      <c r="J12" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="K12" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="L12" s="8">
+        <v>2</v>
+      </c>
+      <c r="M12" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="N12" s="5"/>
+      <c r="P12">
+        <f>F12/G12</f>
         <v>1</v>
       </c>
-      <c r="L12">
-        <f t="shared" si="1"/>
+      <c r="Q12">
+        <f>4*F12</f>
         <v>12</v>
       </c>
-      <c r="N12">
-        <f t="shared" si="2"/>
+      <c r="S12">
+        <f>C12/D12</f>
         <v>1.375</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -990,21 +1189,36 @@
       <c r="H13" s="5">
         <v>8</v>
       </c>
-      <c r="I13" s="5"/>
-      <c r="K13">
-        <f t="shared" si="0"/>
+      <c r="I13" s="8">
+        <v>53</v>
+      </c>
+      <c r="J13" s="8">
+        <v>6</v>
+      </c>
+      <c r="K13" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="L13" s="8">
+        <v>4</v>
+      </c>
+      <c r="M13" s="8">
+        <v>2</v>
+      </c>
+      <c r="N13" s="5"/>
+      <c r="P13">
+        <f>F13/G13</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L13">
-        <f t="shared" si="1"/>
+      <c r="Q13">
+        <f>4*F13</f>
         <v>28</v>
       </c>
-      <c r="N13">
-        <f t="shared" si="2"/>
+      <c r="S13">
+        <f>C13/D13</f>
         <v>1.5294117647058822</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1029,15 +1243,30 @@
       <c r="H14" s="5">
         <v>0</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="8">
+        <v>50</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="8">
+        <v>2</v>
+      </c>
+      <c r="L14" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="M14" s="8">
+        <v>1</v>
+      </c>
+      <c r="N14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="N14">
-        <f t="shared" si="2"/>
+      <c r="S14">
+        <f>C14/D14</f>
         <v>1.4</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>15</v>
       </c>
@@ -1062,15 +1291,30 @@
       <c r="H15" s="5">
         <v>1</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="8">
+        <v>48</v>
+      </c>
+      <c r="J15" s="8">
+        <v>4</v>
+      </c>
+      <c r="K15" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="L15" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="M15" s="8">
+        <v>1</v>
+      </c>
+      <c r="N15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="N15">
-        <f t="shared" si="2"/>
+      <c r="S15">
+        <f>C15/D15</f>
         <v>1.8181818181818181</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>17</v>
       </c>
@@ -1095,21 +1339,36 @@
       <c r="H16" s="5">
         <v>6</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="K16">
-        <f t="shared" si="0"/>
+      <c r="I16" s="8">
+        <v>50</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="8">
+        <v>3</v>
+      </c>
+      <c r="L16" s="8">
+        <v>3</v>
+      </c>
+      <c r="M16" s="8">
+        <v>1</v>
+      </c>
+      <c r="N16" s="5"/>
+      <c r="P16">
+        <f>F16/G16</f>
         <v>1.25</v>
       </c>
-      <c r="L16">
-        <f t="shared" si="1"/>
+      <c r="Q16">
+        <f>4*F16</f>
         <v>20</v>
       </c>
-      <c r="N16">
-        <f t="shared" si="2"/>
+      <c r="S16">
+        <f>C16/D16</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>18</v>
       </c>
@@ -1134,23 +1393,38 @@
       <c r="H17" s="5">
         <v>2</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="8">
+        <v>50</v>
+      </c>
+      <c r="J17" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="K17" s="8">
+        <v>4</v>
+      </c>
+      <c r="L17" s="8">
+        <v>3.8</v>
+      </c>
+      <c r="M17" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="N17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="0"/>
+      <c r="P17">
+        <f>F17/G17</f>
         <v>1</v>
       </c>
-      <c r="L17">
-        <f t="shared" si="1"/>
+      <c r="Q17">
+        <f>4*F17</f>
         <v>20</v>
       </c>
-      <c r="N17">
-        <f t="shared" si="2"/>
+      <c r="S17">
+        <f>C17/D17</f>
         <v>0.9642857142857143</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>20</v>
       </c>
@@ -1175,23 +1449,38 @@
       <c r="H18" s="5">
         <v>7</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="8">
+        <v>68</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K18">
-        <f t="shared" si="0"/>
+      <c r="P18">
+        <f>F18/G18</f>
         <v>1</v>
       </c>
-      <c r="L18">
-        <f t="shared" si="1"/>
+      <c r="Q18">
+        <f>4*F18</f>
         <v>12</v>
       </c>
-      <c r="N18">
-        <f t="shared" si="2"/>
+      <c r="S18">
+        <f>C18/D18</f>
         <v>1.4444444444444444</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>21</v>
       </c>
@@ -1216,21 +1505,36 @@
       <c r="H19" s="5">
         <v>6</v>
       </c>
-      <c r="I19" s="5"/>
-      <c r="K19">
-        <f t="shared" si="0"/>
+      <c r="I19" s="8">
+        <v>45</v>
+      </c>
+      <c r="J19" s="8">
+        <v>7</v>
+      </c>
+      <c r="K19" s="10">
+        <v>4</v>
+      </c>
+      <c r="L19" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="M19" s="9">
+        <v>1</v>
+      </c>
+      <c r="N19" s="5"/>
+      <c r="P19">
+        <f>F19/G19</f>
         <v>1.5</v>
       </c>
-      <c r="L19">
-        <f t="shared" si="1"/>
+      <c r="Q19">
+        <f>4*F19</f>
         <v>24</v>
       </c>
-      <c r="N19">
-        <f t="shared" si="2"/>
+      <c r="S19">
+        <f>C19/D19</f>
         <v>1.8235294117647058</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>22</v>
       </c>
@@ -1255,15 +1559,30 @@
       <c r="H20" s="5">
         <v>2</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="8">
+        <v>45</v>
+      </c>
+      <c r="J20" s="8">
+        <v>4</v>
+      </c>
+      <c r="K20" s="10">
+        <v>4.5</v>
+      </c>
+      <c r="L20" s="9">
+        <v>3</v>
+      </c>
+      <c r="M20" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="N20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="N20">
-        <f t="shared" si="2"/>
+      <c r="S20">
+        <f>C20/D20</f>
         <v>1.7647058823529411</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>23</v>
       </c>
@@ -1288,11 +1607,26 @@
       <c r="H21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N21" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>25</v>
       </c>
@@ -1317,15 +1651,30 @@
       <c r="H22" s="5">
         <v>0</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I22" s="8">
+        <v>50</v>
+      </c>
+      <c r="J22" s="8">
+        <v>4</v>
+      </c>
+      <c r="K22" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="L22" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="M22" s="8">
+        <v>1</v>
+      </c>
+      <c r="N22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="N22">
-        <f t="shared" si="2"/>
+      <c r="S22">
+        <f>C22/D22</f>
         <v>2.4</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>26</v>
       </c>
@@ -1350,15 +1699,30 @@
       <c r="H23" s="5">
         <v>0</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="8">
+        <v>45</v>
+      </c>
+      <c r="J23" s="8">
+        <v>4</v>
+      </c>
+      <c r="K23" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="L23" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="M23" s="8">
+        <v>1</v>
+      </c>
+      <c r="N23" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="N23">
-        <f t="shared" si="2"/>
+      <c r="S23">
+        <f>C23/D23</f>
         <v>1.4285714285714286</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>27</v>
       </c>
@@ -1383,42 +1747,57 @@
       <c r="H24" s="5">
         <v>9</v>
       </c>
-      <c r="I24" s="5"/>
-      <c r="K24">
-        <f t="shared" si="0"/>
+      <c r="I24" s="8">
+        <v>35</v>
+      </c>
+      <c r="J24" s="8">
+        <v>5</v>
+      </c>
+      <c r="K24" s="8">
+        <v>4.2</v>
+      </c>
+      <c r="L24" s="8">
+        <v>5</v>
+      </c>
+      <c r="M24" s="8">
+        <v>2</v>
+      </c>
+      <c r="N24" s="5"/>
+      <c r="P24">
+        <f>F24/G24</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L24">
-        <f t="shared" si="1"/>
+      <c r="Q24">
+        <f>4*F24</f>
         <v>28</v>
       </c>
-      <c r="N24">
-        <f t="shared" si="2"/>
+      <c r="S24">
+        <f>C24/D24</f>
         <v>2.6153846153846154</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J25" s="1" t="s">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K25">
-        <f>AVERAGE(K2:K24)</f>
+      <c r="P25">
+        <f>AVERAGE(P2:P24)</f>
         <v>1.175</v>
       </c>
-      <c r="L25">
-        <f>AVERAGE(L2:L24)</f>
+      <c r="Q25">
+        <f>AVERAGE(Q2:Q24)</f>
         <v>19.25</v>
       </c>
-      <c r="N25">
-        <f>AVERAGE(N2:N24)</f>
+      <c r="S25">
+        <f>AVERAGE(S2:S24)</f>
         <v>1.5732710753298988</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="K26" t="s">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P26" t="s">
         <v>21</v>
       </c>
-      <c r="L26" t="s">
+      <c r="Q26" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Shirt + Head template AND RW Image
</commit_message>
<xml_diff>
--- a/template/features.xlsx
+++ b/template/features.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9672"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9672" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="31">
   <si>
     <t>Image</t>
   </si>
@@ -111,6 +112,12 @@
   </si>
   <si>
     <t>Angle beanie (compared to horizontal, always tilted in same direction)</t>
+  </si>
+  <si>
+    <t>Corr:</t>
+  </si>
+  <si>
+    <t>Relationship between stripe height in the shirt and red stripe in hat</t>
   </si>
 </sst>
 </file>
@@ -214,6 +221,2039 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil2!$A$1:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6A2A-451C-9C85-12E505FA9FF1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil2!$B$1:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6A2A-451C-9C85-12E505FA9FF1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="399638440"/>
+        <c:axId val="399638112"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="399638440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="399638112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="399638112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="399638440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.0232939632545932E-2"/>
+                  <c:y val="-0.22410323709536309"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil2!$A$1:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil2!$B$1:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8095-4D51-BE4B-BFBA43005F94}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="402812648"/>
+        <c:axId val="402812976"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="402812648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="402812976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="402812976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="402812648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEC3427F-D80B-450C-9565-76A173B3D009}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6ABE9671-CBE0-4F9D-8F14-C95EBA89FD15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -513,11 +2553,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J24" sqref="J24"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,7 +2565,7 @@
     <col min="1" max="6" width="25.77734375" customWidth="1"/>
     <col min="7" max="7" width="21.33203125" customWidth="1"/>
     <col min="8" max="8" width="25.77734375" customWidth="1"/>
-    <col min="9" max="9" width="20.21875" customWidth="1"/>
+    <col min="9" max="9" width="31.77734375" customWidth="1"/>
     <col min="10" max="10" width="46.109375" customWidth="1"/>
     <col min="11" max="13" width="30.88671875" customWidth="1"/>
     <col min="14" max="14" width="17.109375" customWidth="1"/>
@@ -533,7 +2573,7 @@
     <col min="16" max="16" width="35.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -587,7 +2627,7 @@
       </c>
       <c r="T1" s="6"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -629,19 +2669,23 @@
       </c>
       <c r="N2" s="5"/>
       <c r="P2">
-        <f>F2/G2</f>
+        <f t="shared" ref="P2:P7" si="0">F2/G2</f>
         <v>1.5</v>
       </c>
       <c r="Q2">
-        <f>4*F2</f>
+        <f t="shared" ref="Q2:Q7" si="1">4*F2</f>
         <v>12</v>
       </c>
       <c r="S2">
-        <f>C2/D2</f>
+        <f t="shared" ref="S2:S7" si="2">C2/D2</f>
         <v>1.1666666666666667</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="V2">
+        <f>CORREL(F2:F24,L2:L24)</f>
+        <v>0.76336658189512729</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -685,19 +2729,19 @@
         <v>12</v>
       </c>
       <c r="P3">
-        <f>F3/G3</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q3">
-        <f>4*F3</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="S3">
-        <f>C3/D3</f>
+        <f t="shared" si="2"/>
         <v>1.2727272727272727</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -739,19 +2783,19 @@
       </c>
       <c r="N4" s="5"/>
       <c r="P4">
-        <f>F4/G4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q4">
-        <f>4*F4</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="S4">
-        <f>C4/D4</f>
+        <f t="shared" si="2"/>
         <v>1.4545454545454546</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -793,19 +2837,19 @@
       </c>
       <c r="N5" s="5"/>
       <c r="P5">
-        <f>F5/G5</f>
+        <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="Q5">
-        <f>4*F5</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="S5">
-        <f>C5/D5</f>
+        <f t="shared" si="2"/>
         <v>1.6</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -847,19 +2891,19 @@
       </c>
       <c r="N6" s="5"/>
       <c r="P6">
-        <f>F6/G6</f>
+        <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="Q6">
-        <f>4*F6</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="S6">
-        <f>C6/D6</f>
+        <f t="shared" si="2"/>
         <v>1.5714285714285714</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -903,19 +2947,19 @@
         <v>10</v>
       </c>
       <c r="P7">
-        <f>F7/G7</f>
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="Q7">
-        <f>4*F7</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="S7">
-        <f>C7/D7</f>
+        <f t="shared" si="2"/>
         <v>1.4615384615384615</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -962,7 +3006,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1006,7 +3050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1052,11 +3096,11 @@
         <v>16</v>
       </c>
       <c r="S10">
-        <f>C10/D10</f>
+        <f t="shared" ref="S10:S20" si="3">C10/D10</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1106,11 +3150,11 @@
         <v>12</v>
       </c>
       <c r="S11">
-        <f>C11/D11</f>
+        <f t="shared" si="3"/>
         <v>1.375</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1160,11 +3204,11 @@
         <v>12</v>
       </c>
       <c r="S12">
-        <f>C12/D12</f>
+        <f t="shared" si="3"/>
         <v>1.375</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1214,11 +3258,11 @@
         <v>28</v>
       </c>
       <c r="S13">
-        <f>C13/D13</f>
+        <f t="shared" si="3"/>
         <v>1.5294117647058822</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1262,11 +3306,11 @@
         <v>15</v>
       </c>
       <c r="S14">
-        <f>C14/D14</f>
+        <f t="shared" si="3"/>
         <v>1.4</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>15</v>
       </c>
@@ -1310,11 +3354,11 @@
         <v>16</v>
       </c>
       <c r="S15">
-        <f>C15/D15</f>
+        <f t="shared" si="3"/>
         <v>1.8181818181818181</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>17</v>
       </c>
@@ -1364,7 +3408,7 @@
         <v>20</v>
       </c>
       <c r="S16">
-        <f>C16/D16</f>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1420,7 +3464,7 @@
         <v>20</v>
       </c>
       <c r="S17">
-        <f>C17/D17</f>
+        <f t="shared" si="3"/>
         <v>0.9642857142857143</v>
       </c>
     </row>
@@ -1476,7 +3520,7 @@
         <v>12</v>
       </c>
       <c r="S18">
-        <f>C18/D18</f>
+        <f t="shared" si="3"/>
         <v>1.4444444444444444</v>
       </c>
     </row>
@@ -1530,7 +3574,7 @@
         <v>24</v>
       </c>
       <c r="S19">
-        <f>C19/D19</f>
+        <f t="shared" si="3"/>
         <v>1.8235294117647058</v>
       </c>
     </row>
@@ -1578,7 +3622,7 @@
         <v>16</v>
       </c>
       <c r="S20">
-        <f>C20/D20</f>
+        <f t="shared" si="3"/>
         <v>1.7647058823529411</v>
       </c>
     </row>
@@ -1805,4 +3849,144 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="5">
+        <v>3</v>
+      </c>
+      <c r="B1" s="8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1">
+        <f>CORREL(A1:A14,B1:B14)</f>
+        <v>0.91798801217464798</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>3</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>3</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>3</v>
+      </c>
+      <c r="B9" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>7</v>
+      </c>
+      <c r="B10" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>5</v>
+      </c>
+      <c r="B11" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>5</v>
+      </c>
+      <c r="B12" s="8">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>6</v>
+      </c>
+      <c r="B13" s="9">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>7</v>
+      </c>
+      <c r="B14" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>